<commit_message>
Modify store and product excel files.
</commit_message>
<xml_diff>
--- a/product.xlsx
+++ b/product.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paris\Documents\Jane\git-demo-sbareh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paris\Documents\Jane\git-real\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Product</t>
   </si>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>Photo</t>
+  </si>
+  <si>
+    <t>nuts</t>
+  </si>
+  <si>
+    <t>honey</t>
+  </si>
+  <si>
+    <t>fruits</t>
+  </si>
+  <si>
+    <t>breads</t>
   </si>
 </sst>
 </file>
@@ -365,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,6 +418,26 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>

</xml_diff>

<commit_message>
Add pain relief pills
</commit_message>
<xml_diff>
--- a/product.xlsx
+++ b/product.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Product</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>breads</t>
+  </si>
+  <si>
+    <t>Pain relief pills</t>
   </si>
 </sst>
 </file>
@@ -380,12 +383,13 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -426,6 +430,9 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>